<commit_message>
Changed the rent amount
</commit_message>
<xml_diff>
--- a/Budgeting Spreadsheet Heather_Andre.xlsx
+++ b/Budgeting Spreadsheet Heather_Andre.xlsx
@@ -1011,51 +1011,51 @@
         <v>43</v>
       </c>
       <c r="B11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" ref="B11:M11" si="3">465+293+85</f>
         <v>843</v>
       </c>
       <c r="C11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="D11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="E11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="F11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="G11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="H11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="I11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="J11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="K11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="L11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="M11" s="3">
-        <f>465+293+85</f>
+        <f t="shared" si="3"/>
         <v>843</v>
       </c>
       <c r="N11" s="3">
@@ -1207,47 +1207,47 @@
         <v>4470</v>
       </c>
       <c r="C15" s="6">
-        <f t="shared" ref="C15:M15" si="3">SUM(C9:C14)</f>
+        <f t="shared" ref="C15:M15" si="4">SUM(C9:C14)</f>
         <v>4470</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4470</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4470</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4470</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4470</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4920</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4920</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4470</v>
       </c>
       <c r="K15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4470</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4470</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4470</v>
       </c>
       <c r="N15" s="6">
@@ -1263,51 +1263,51 @@
         <v>0.44367245657568238</v>
       </c>
       <c r="C16" s="4">
-        <f t="shared" ref="C16:N16" si="4">IF(C$7=0,0,C15/C$7)</f>
+        <f t="shared" ref="C16:N16" si="5">IF(C$7=0,0,C15/C$7)</f>
         <v>0.44367245657568238</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.44367245657568238</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.44367245657568238</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.38617710583153347</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.44367245657568238</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.48833746898263025</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.48833746898263025</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.44367245657568238</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.38617710583153347</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.44367245657568238</v>
       </c>
       <c r="M16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.27198052935807726</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.41870105941962227</v>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
         <v>1200</v>
       </c>
       <c r="N19" s="3">
-        <f t="shared" ref="N19:N23" si="5">SUM(B19:M19)</f>
+        <f t="shared" ref="N19:N23" si="6">SUM(B19:M19)</f>
         <v>14400</v>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
         <v>110</v>
       </c>
       <c r="N20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1320</v>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
         <v>400</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4800</v>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
         <v>100</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1200</v>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
         <v>1150</v>
       </c>
       <c r="N23" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13800</v>
       </c>
     </row>
@@ -1575,55 +1575,55 @@
         <v>29</v>
       </c>
       <c r="B24" s="6">
-        <f>SUM(B18:B23)</f>
+        <f t="shared" ref="B24:N24" si="7">SUM(B18:B23)</f>
         <v>2960</v>
       </c>
       <c r="C24" s="6">
-        <f>SUM(C18:C23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="D24" s="6">
-        <f>SUM(D18:D23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="E24" s="6">
-        <f>SUM(E18:E23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="F24" s="6">
-        <f>SUM(F18:F23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="G24" s="6">
-        <f>SUM(G18:G23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="H24" s="6">
-        <f>SUM(H18:H23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="I24" s="6">
-        <f>SUM(I18:I23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="J24" s="6">
-        <f>SUM(J18:J23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="K24" s="6">
-        <f>SUM(K18:K23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="L24" s="6">
-        <f>SUM(L18:L23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="M24" s="6">
-        <f>SUM(M18:M23)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
       <c r="N24" s="6">
-        <f>SUM(N18:N23)</f>
+        <f t="shared" si="7"/>
         <v>35520</v>
       </c>
       <c r="P24" s="1"/>
@@ -1635,51 +1635,51 @@
         <v>0.29379652605459056</v>
       </c>
       <c r="C25" s="4">
-        <f t="shared" ref="C25:N25" si="6">IF(C$7=0,0,C24/C$7)</f>
+        <f t="shared" ref="C25:N25" si="8">IF(C$7=0,0,C24/C$7)</f>
         <v>0.29379652605459056</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.29379652605459056</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.29379652605459056</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.25572354211663068</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.29379652605459056</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.29379652605459056</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.29379652605459056</v>
       </c>
       <c r="J25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.29379652605459056</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.25572354211663068</v>
       </c>
       <c r="L25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.29379652605459056</v>
       </c>
       <c r="M25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.18010343778521448</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.27268539843390144</v>
       </c>
     </row>
@@ -1758,7 +1758,7 @@
         <v>290</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" ref="N28:N40" si="7">SUM(B28:M28)</f>
+        <f t="shared" ref="N28:N40" si="9">SUM(B28:M28)</f>
         <v>3480</v>
       </c>
     </row>
@@ -1803,7 +1803,7 @@
         <v>400</v>
       </c>
       <c r="N29" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4800</v>
       </c>
     </row>
@@ -1848,7 +1848,7 @@
         <v>160</v>
       </c>
       <c r="N30" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1920</v>
       </c>
     </row>
@@ -1893,7 +1893,7 @@
         <v>70</v>
       </c>
       <c r="N31" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>840</v>
       </c>
     </row>
@@ -1938,7 +1938,7 @@
         <v>15</v>
       </c>
       <c r="N32" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>180</v>
       </c>
     </row>
@@ -1983,7 +1983,7 @@
         <v>100</v>
       </c>
       <c r="N33" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1200</v>
       </c>
     </row>
@@ -2028,7 +2028,7 @@
         <v>80</v>
       </c>
       <c r="N34" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>960</v>
       </c>
     </row>
@@ -2073,7 +2073,7 @@
         <v>240</v>
       </c>
       <c r="N35" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2880</v>
       </c>
     </row>
@@ -2118,7 +2118,7 @@
         <v>160</v>
       </c>
       <c r="N36" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1920</v>
       </c>
     </row>
@@ -2163,7 +2163,7 @@
         <v>150</v>
       </c>
       <c r="N37" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1800</v>
       </c>
     </row>
@@ -2208,7 +2208,7 @@
         <v>200</v>
       </c>
       <c r="N38" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2400</v>
       </c>
     </row>
@@ -2253,7 +2253,7 @@
         <v>260</v>
       </c>
       <c r="N39" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3120</v>
       </c>
     </row>
@@ -2310,7 +2310,7 @@
         <v>200</v>
       </c>
       <c r="N40" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3100</v>
       </c>
     </row>
@@ -2323,47 +2323,47 @@
         <v>2325</v>
       </c>
       <c r="C41" s="6">
-        <f t="shared" ref="C41:M41" si="8">SUM(C28:C40)</f>
+        <f t="shared" ref="C41:M41" si="10">SUM(C28:C40)</f>
         <v>2325</v>
       </c>
       <c r="D41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2325</v>
       </c>
       <c r="E41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2325</v>
       </c>
       <c r="F41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2325</v>
       </c>
       <c r="G41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2325</v>
       </c>
       <c r="H41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2325</v>
       </c>
       <c r="I41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2325</v>
       </c>
       <c r="J41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2325</v>
       </c>
       <c r="K41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2325</v>
       </c>
       <c r="L41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3025</v>
       </c>
       <c r="M41" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2325</v>
       </c>
       <c r="N41" s="6">
@@ -2379,51 +2379,51 @@
         <v>0.23076923076923078</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" ref="C42:N42" si="9">IF(C$7=0,0,C41/C$7)</f>
+        <f t="shared" ref="C42:N42" si="11">IF(C$7=0,0,C41/C$7)</f>
         <v>0.23076923076923078</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.20086393088552915</v>
       </c>
       <c r="G42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="I42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="J42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.20086393088552915</v>
       </c>
       <c r="L42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.30024813895781638</v>
       </c>
       <c r="M42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.1414663827198053</v>
       </c>
       <c r="N42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.21956087824351297</v>
       </c>
     </row>
@@ -2464,55 +2464,55 @@
         <v>31</v>
       </c>
       <c r="B45" s="3">
-        <f>B15+B24+B41</f>
+        <f t="shared" ref="B45:N45" si="12">B15+B24+B41</f>
         <v>9755</v>
       </c>
       <c r="C45" s="3">
-        <f>C15+C24+C41</f>
+        <f t="shared" si="12"/>
         <v>9755</v>
       </c>
       <c r="D45" s="3">
-        <f>D15+D24+D41</f>
+        <f t="shared" si="12"/>
         <v>9755</v>
       </c>
       <c r="E45" s="3">
-        <f>E15+E24+E41</f>
+        <f t="shared" si="12"/>
         <v>9755</v>
       </c>
       <c r="F45" s="3">
-        <f>F15+F24+F41</f>
+        <f t="shared" si="12"/>
         <v>9755</v>
       </c>
       <c r="G45" s="3">
-        <f>G15+G24+G41</f>
+        <f t="shared" si="12"/>
         <v>9755</v>
       </c>
       <c r="H45" s="3">
-        <f>H15+H24+H41</f>
+        <f t="shared" si="12"/>
         <v>10205</v>
       </c>
       <c r="I45" s="3">
-        <f>I15+I24+I41</f>
+        <f t="shared" si="12"/>
         <v>10205</v>
       </c>
       <c r="J45" s="3">
-        <f>J15+J24+J41</f>
+        <f t="shared" si="12"/>
         <v>9755</v>
       </c>
       <c r="K45" s="3">
-        <f>K15+K24+K41</f>
+        <f t="shared" si="12"/>
         <v>9755</v>
       </c>
       <c r="L45" s="3">
-        <f>L15+L24+L41</f>
+        <f t="shared" si="12"/>
         <v>10455</v>
       </c>
       <c r="M45" s="3">
-        <f>M15+M24+M41</f>
+        <f t="shared" si="12"/>
         <v>9755</v>
       </c>
       <c r="N45" s="3">
-        <f>N15+N24+N41</f>
+        <f t="shared" si="12"/>
         <v>118660</v>
       </c>
     </row>
@@ -2523,51 +2523,51 @@
         <v>0.96823821339950367</v>
       </c>
       <c r="C46" s="4">
-        <f t="shared" ref="C46:N46" si="10">IF(C$7=0,0,C45/C$7)</f>
+        <f t="shared" ref="C46:N46" si="13">IF(C$7=0,0,C45/C$7)</f>
         <v>0.96823821339950367</v>
       </c>
       <c r="D46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.96823821339950367</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.96823821339950367</v>
       </c>
       <c r="F46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.84276457883369327</v>
       </c>
       <c r="G46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.96823821339950367</v>
       </c>
       <c r="H46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.0129032258064516</v>
       </c>
       <c r="I46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.0129032258064516</v>
       </c>
       <c r="J46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.96823821339950367</v>
       </c>
       <c r="K46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.84276457883369327</v>
       </c>
       <c r="L46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.0377171215880894</v>
       </c>
       <c r="M46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.59355034986309707</v>
       </c>
       <c r="N46" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.91094733609703671</v>
       </c>
     </row>
@@ -2592,55 +2592,55 @@
         <v>26</v>
       </c>
       <c r="B48" s="6">
-        <f>B7-B45</f>
+        <f t="shared" ref="B48:N48" si="14">B7-B45</f>
         <v>320</v>
       </c>
       <c r="C48" s="6">
-        <f>C7-C45</f>
+        <f t="shared" si="14"/>
         <v>320</v>
       </c>
       <c r="D48" s="6">
-        <f>D7-D45</f>
+        <f t="shared" si="14"/>
         <v>320</v>
       </c>
       <c r="E48" s="6">
-        <f>E7-E45</f>
+        <f t="shared" si="14"/>
         <v>320</v>
       </c>
       <c r="F48" s="6">
-        <f>F7-F45</f>
+        <f t="shared" si="14"/>
         <v>1820</v>
       </c>
       <c r="G48" s="6">
-        <f>G7-G45</f>
+        <f t="shared" si="14"/>
         <v>320</v>
       </c>
       <c r="H48" s="6">
-        <f>H7-H45</f>
+        <f t="shared" si="14"/>
         <v>-130</v>
       </c>
       <c r="I48" s="6">
-        <f>I7-I45</f>
+        <f t="shared" si="14"/>
         <v>-130</v>
       </c>
       <c r="J48" s="6">
-        <f>J7-J45</f>
+        <f t="shared" si="14"/>
         <v>320</v>
       </c>
       <c r="K48" s="6">
-        <f>K7-K45</f>
+        <f t="shared" si="14"/>
         <v>1820</v>
       </c>
       <c r="L48" s="6">
-        <f>L7-L45</f>
+        <f t="shared" si="14"/>
         <v>-380</v>
       </c>
       <c r="M48" s="6">
-        <f>M7-M45</f>
+        <f t="shared" si="14"/>
         <v>6680</v>
       </c>
       <c r="N48" s="6">
-        <f>N7-N45</f>
+        <f t="shared" si="14"/>
         <v>11600</v>
       </c>
     </row>
@@ -2651,51 +2651,51 @@
         <v>3.1761786600496278E-2</v>
       </c>
       <c r="C49" s="4">
-        <f t="shared" ref="C49:N49" si="11">IF(C$7=0,0,C48/C$7)</f>
+        <f t="shared" ref="C49:N49" si="15">IF(C$7=0,0,C48/C$7)</f>
         <v>3.1761786600496278E-2</v>
       </c>
       <c r="D49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>3.1761786600496278E-2</v>
       </c>
       <c r="E49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>3.1761786600496278E-2</v>
       </c>
       <c r="F49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.1572354211663067</v>
       </c>
       <c r="G49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>3.1761786600496278E-2</v>
       </c>
       <c r="H49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>-1.2903225806451613E-2</v>
       </c>
       <c r="I49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>-1.2903225806451613E-2</v>
       </c>
       <c r="J49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>3.1761786600496278E-2</v>
       </c>
       <c r="K49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.1572354211663067</v>
       </c>
       <c r="L49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>-3.7717121588089333E-2</v>
       </c>
       <c r="M49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.40644965013690293</v>
       </c>
       <c r="N49" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>8.9052663902963305E-2</v>
       </c>
     </row>
@@ -5032,7 +5032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5312,44 +5314,44 @@
         <v>38</v>
       </c>
       <c r="B9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="C9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="D9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="E9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="F9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="G9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="H9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="I9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="J9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="K9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="L9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="M9" s="3">
-        <v>1780</v>
+        <v>1800</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="2"/>
-        <v>21360</v>
+        <v>21600</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1">
@@ -5357,51 +5359,51 @@
         <v>43</v>
       </c>
       <c r="B10" s="3">
-        <f>293+85</f>
+        <f t="shared" ref="B10:M10" si="3">293+85</f>
         <v>378</v>
       </c>
       <c r="C10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="D10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="E10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="F10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="G10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="H10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="I10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="J10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="K10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="L10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="M10" s="3">
-        <f>293+85</f>
+        <f t="shared" si="3"/>
         <v>378</v>
       </c>
       <c r="N10" s="3">
@@ -5504,111 +5506,111 @@
         <v>28</v>
       </c>
       <c r="B13" s="6">
-        <f t="shared" ref="B13:N13" si="3">SUM(B8:B12)</f>
-        <v>2908</v>
+        <f t="shared" ref="B13:N13" si="4">SUM(B8:B12)</f>
+        <v>2928</v>
       </c>
       <c r="C13" s="6">
-        <f t="shared" si="3"/>
-        <v>2908</v>
+        <f t="shared" si="4"/>
+        <v>2928</v>
       </c>
       <c r="D13" s="6">
-        <f t="shared" si="3"/>
-        <v>2908</v>
+        <f t="shared" si="4"/>
+        <v>2928</v>
       </c>
       <c r="E13" s="6">
-        <f t="shared" si="3"/>
-        <v>2908</v>
+        <f t="shared" si="4"/>
+        <v>2928</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="3"/>
-        <v>2908</v>
+        <f t="shared" si="4"/>
+        <v>2928</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="3"/>
-        <v>2908</v>
+        <f t="shared" si="4"/>
+        <v>2928</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="3"/>
-        <v>3358</v>
+        <f t="shared" si="4"/>
+        <v>3378</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="3"/>
-        <v>3358</v>
+        <f t="shared" si="4"/>
+        <v>3378</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="3"/>
-        <v>2908</v>
+        <f t="shared" si="4"/>
+        <v>2928</v>
       </c>
       <c r="K13" s="6">
-        <f t="shared" si="3"/>
-        <v>2908</v>
+        <f t="shared" si="4"/>
+        <v>2928</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="3"/>
-        <v>2908</v>
+        <f t="shared" si="4"/>
+        <v>2928</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="3"/>
-        <v>2908</v>
+        <f t="shared" si="4"/>
+        <v>2928</v>
       </c>
       <c r="N13" s="6">
-        <f t="shared" si="3"/>
-        <v>35796</v>
+        <f t="shared" si="4"/>
+        <v>36036</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1">
       <c r="A14" s="11"/>
       <c r="B14" s="4">
         <f>IF(B$6=0,0,B13/B$6)</f>
-        <v>0.52872727272727271</v>
+        <v>0.53236363636363637</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" ref="C14:N14" si="4">IF(C$6=0,0,C13/C$6)</f>
-        <v>0.52872727272727271</v>
+        <f t="shared" ref="C14:N14" si="5">IF(C$6=0,0,C13/C$6)</f>
+        <v>0.53236363636363637</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.52872727272727271</v>
+        <f t="shared" si="5"/>
+        <v>0.53236363636363637</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.52872727272727271</v>
+        <f t="shared" si="5"/>
+        <v>0.53236363636363637</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.52872727272727271</v>
+        <f t="shared" si="5"/>
+        <v>0.53236363636363637</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.52872727272727271</v>
+        <f t="shared" si="5"/>
+        <v>0.53236363636363637</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.6105454545454545</v>
+        <f t="shared" si="5"/>
+        <v>0.61418181818181816</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.6105454545454545</v>
+        <f t="shared" si="5"/>
+        <v>0.61418181818181816</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.52872727272727271</v>
+        <f t="shared" si="5"/>
+        <v>0.53236363636363637</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.52872727272727271</v>
+        <f t="shared" si="5"/>
+        <v>0.53236363636363637</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.52872727272727271</v>
+        <f t="shared" si="5"/>
+        <v>0.53236363636363637</v>
       </c>
       <c r="M14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.24519392917369309</v>
+        <f t="shared" si="5"/>
+        <v>0.24688026981450253</v>
       </c>
       <c r="N14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.49469320066334993</v>
+        <f t="shared" si="5"/>
+        <v>0.49800995024875622</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="1" customFormat="1">
@@ -5686,7 +5688,7 @@
         <v>575</v>
       </c>
       <c r="N17" s="3">
-        <f t="shared" ref="N17:N21" si="5">SUM(B17:M17)</f>
+        <f t="shared" ref="N17:N21" si="6">SUM(B17:M17)</f>
         <v>6900</v>
       </c>
     </row>
@@ -5731,7 +5733,7 @@
         <v>55</v>
       </c>
       <c r="N18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>660</v>
       </c>
     </row>
@@ -5776,7 +5778,7 @@
         <v>200</v>
       </c>
       <c r="N19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2400</v>
       </c>
     </row>
@@ -5821,7 +5823,7 @@
         <v>50</v>
       </c>
       <c r="N20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>600</v>
       </c>
     </row>
@@ -5866,7 +5868,7 @@
         <v>500</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6000</v>
       </c>
     </row>
@@ -5875,55 +5877,55 @@
         <v>29</v>
       </c>
       <c r="B22" s="6">
-        <f t="shared" ref="B22:N22" si="6">SUM(B16:B21)</f>
+        <f t="shared" ref="B22:N22" si="7">SUM(B16:B21)</f>
         <v>1380</v>
       </c>
       <c r="C22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="D22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="E22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="G22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="H22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="I22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="J22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="K22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="L22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="M22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1380</v>
       </c>
       <c r="N22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16560</v>
       </c>
     </row>
@@ -5934,51 +5936,51 @@
         <v>0.25090909090909091</v>
       </c>
       <c r="C23" s="4">
-        <f t="shared" ref="C23:N23" si="7">IF(C$6=0,0,C22/C$6)</f>
+        <f t="shared" ref="C23:N23" si="8">IF(C$6=0,0,C22/C$6)</f>
         <v>0.25090909090909091</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25090909090909091</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25090909090909091</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25090909090909091</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25090909090909091</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25090909090909091</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25090909090909091</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25090909090909091</v>
       </c>
       <c r="K23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25090909090909091</v>
       </c>
       <c r="L23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25090909090909091</v>
       </c>
       <c r="M23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1163575042158516</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.22885572139303484</v>
       </c>
     </row>
@@ -6057,7 +6059,7 @@
         <v>145</v>
       </c>
       <c r="N26" s="3">
-        <f t="shared" ref="N26:N37" si="8">SUM(B26:M26)</f>
+        <f t="shared" ref="N26:N37" si="9">SUM(B26:M26)</f>
         <v>1740</v>
       </c>
     </row>
@@ -6102,7 +6104,7 @@
         <v>200</v>
       </c>
       <c r="N27" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2400</v>
       </c>
     </row>
@@ -6147,7 +6149,7 @@
         <v>80</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>960</v>
       </c>
     </row>
@@ -6192,7 +6194,7 @@
         <v>35</v>
       </c>
       <c r="N29" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>420</v>
       </c>
     </row>
@@ -6213,7 +6215,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6258,7 +6260,7 @@
         <v>50</v>
       </c>
       <c r="N31" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>600</v>
       </c>
     </row>
@@ -6303,7 +6305,7 @@
         <v>40</v>
       </c>
       <c r="N32" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>480</v>
       </c>
     </row>
@@ -6348,7 +6350,7 @@
         <v>120</v>
       </c>
       <c r="N33" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1440</v>
       </c>
     </row>
@@ -6393,7 +6395,7 @@
         <v>80</v>
       </c>
       <c r="N34" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>960</v>
       </c>
     </row>
@@ -6438,7 +6440,7 @@
         <v>75</v>
       </c>
       <c r="N35" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>900</v>
       </c>
     </row>
@@ -6483,7 +6485,7 @@
         <v>100</v>
       </c>
       <c r="N36" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1200</v>
       </c>
     </row>
@@ -6528,7 +6530,7 @@
         <v>200</v>
       </c>
       <c r="N37" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2400</v>
       </c>
     </row>
@@ -6537,55 +6539,55 @@
         <v>30</v>
       </c>
       <c r="B38" s="6">
-        <f t="shared" ref="B38:N38" si="9">SUM(B25:B37)</f>
+        <f t="shared" ref="B38:N38" si="10">SUM(B25:B37)</f>
         <v>1125</v>
       </c>
       <c r="C38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="D38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="E38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="F38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="G38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="H38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="I38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="J38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="K38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="L38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="M38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1125</v>
       </c>
       <c r="N38" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13500</v>
       </c>
     </row>
@@ -6596,51 +6598,51 @@
         <v>0.20454545454545456</v>
       </c>
       <c r="C39" s="4">
-        <f t="shared" ref="C39:N39" si="10">IF(C$6=0,0,C38/C$6)</f>
+        <f t="shared" ref="C39:N39" si="11">IF(C$6=0,0,C38/C$6)</f>
         <v>0.20454545454545456</v>
       </c>
       <c r="D39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="F39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="G39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="I39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="J39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="K39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="L39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="M39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.4856661045531199E-2</v>
       </c>
       <c r="N39" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.18656716417910449</v>
       </c>
     </row>
@@ -6681,111 +6683,111 @@
         <v>31</v>
       </c>
       <c r="B42" s="3">
-        <f t="shared" ref="B42:N42" si="11">B13+B22+B38</f>
-        <v>5413</v>
+        <f t="shared" ref="B42:N42" si="12">B13+B22+B38</f>
+        <v>5433</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="11"/>
-        <v>5413</v>
+        <f t="shared" si="12"/>
+        <v>5433</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" si="11"/>
-        <v>5413</v>
+        <f t="shared" si="12"/>
+        <v>5433</v>
       </c>
       <c r="E42" s="3">
-        <f t="shared" si="11"/>
-        <v>5413</v>
+        <f t="shared" si="12"/>
+        <v>5433</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" si="11"/>
-        <v>5413</v>
+        <f t="shared" si="12"/>
+        <v>5433</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" si="11"/>
-        <v>5413</v>
+        <f t="shared" si="12"/>
+        <v>5433</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" si="11"/>
-        <v>5863</v>
+        <f t="shared" si="12"/>
+        <v>5883</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="11"/>
-        <v>5863</v>
+        <f t="shared" si="12"/>
+        <v>5883</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" si="11"/>
-        <v>5413</v>
+        <f t="shared" si="12"/>
+        <v>5433</v>
       </c>
       <c r="K42" s="3">
-        <f t="shared" si="11"/>
-        <v>5413</v>
+        <f t="shared" si="12"/>
+        <v>5433</v>
       </c>
       <c r="L42" s="3">
-        <f t="shared" si="11"/>
-        <v>5413</v>
+        <f t="shared" si="12"/>
+        <v>5433</v>
       </c>
       <c r="M42" s="3">
-        <f t="shared" si="11"/>
-        <v>5413</v>
+        <f t="shared" si="12"/>
+        <v>5433</v>
       </c>
       <c r="N42" s="3">
-        <f t="shared" si="11"/>
-        <v>65856</v>
+        <f t="shared" si="12"/>
+        <v>66096</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="1" customFormat="1">
       <c r="A43" s="9"/>
       <c r="B43" s="4">
         <f>IF(B$6=0,0,B42/B$6)</f>
-        <v>0.98418181818181816</v>
+        <v>0.98781818181818182</v>
       </c>
       <c r="C43" s="4">
-        <f t="shared" ref="C43:N43" si="12">IF(C$6=0,0,C42/C$6)</f>
-        <v>0.98418181818181816</v>
+        <f t="shared" ref="C43:N43" si="13">IF(C$6=0,0,C42/C$6)</f>
+        <v>0.98781818181818182</v>
       </c>
       <c r="D43" s="4">
-        <f t="shared" si="12"/>
-        <v>0.98418181818181816</v>
+        <f t="shared" si="13"/>
+        <v>0.98781818181818182</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="12"/>
-        <v>0.98418181818181816</v>
+        <f t="shared" si="13"/>
+        <v>0.98781818181818182</v>
       </c>
       <c r="F43" s="4">
-        <f t="shared" si="12"/>
-        <v>0.98418181818181816</v>
+        <f t="shared" si="13"/>
+        <v>0.98781818181818182</v>
       </c>
       <c r="G43" s="4">
-        <f t="shared" si="12"/>
-        <v>0.98418181818181816</v>
+        <f t="shared" si="13"/>
+        <v>0.98781818181818182</v>
       </c>
       <c r="H43" s="4">
-        <f t="shared" si="12"/>
-        <v>1.0660000000000001</v>
+        <f t="shared" si="13"/>
+        <v>1.0696363636363637</v>
       </c>
       <c r="I43" s="4">
-        <f t="shared" si="12"/>
-        <v>1.0660000000000001</v>
+        <f t="shared" si="13"/>
+        <v>1.0696363636363637</v>
       </c>
       <c r="J43" s="4">
-        <f t="shared" si="12"/>
-        <v>0.98418181818181816</v>
+        <f t="shared" si="13"/>
+        <v>0.98781818181818182</v>
       </c>
       <c r="K43" s="4">
-        <f t="shared" si="12"/>
-        <v>0.98418181818181816</v>
+        <f t="shared" si="13"/>
+        <v>0.98781818181818182</v>
       </c>
       <c r="L43" s="4">
-        <f t="shared" si="12"/>
-        <v>0.98418181818181816</v>
+        <f t="shared" si="13"/>
+        <v>0.98781818181818182</v>
       </c>
       <c r="M43" s="4">
-        <f t="shared" si="12"/>
-        <v>0.45640809443507591</v>
+        <f t="shared" si="13"/>
+        <v>0.45809443507588532</v>
       </c>
       <c r="N43" s="4">
-        <f t="shared" si="12"/>
-        <v>0.91011608623548923</v>
+        <f t="shared" si="13"/>
+        <v>0.91343283582089552</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="1" customFormat="1">
@@ -6809,111 +6811,111 @@
         <v>26</v>
       </c>
       <c r="B45" s="6">
-        <f t="shared" ref="B45:N45" si="13">B6-B42</f>
-        <v>87</v>
+        <f t="shared" ref="B45:N45" si="14">B6-B42</f>
+        <v>67</v>
       </c>
       <c r="C45" s="6">
-        <f t="shared" si="13"/>
-        <v>87</v>
+        <f t="shared" si="14"/>
+        <v>67</v>
       </c>
       <c r="D45" s="6">
-        <f t="shared" si="13"/>
-        <v>87</v>
+        <f t="shared" si="14"/>
+        <v>67</v>
       </c>
       <c r="E45" s="6">
-        <f t="shared" si="13"/>
-        <v>87</v>
+        <f t="shared" si="14"/>
+        <v>67</v>
       </c>
       <c r="F45" s="6">
-        <f t="shared" si="13"/>
-        <v>87</v>
+        <f t="shared" si="14"/>
+        <v>67</v>
       </c>
       <c r="G45" s="6">
-        <f t="shared" si="13"/>
-        <v>87</v>
+        <f t="shared" si="14"/>
+        <v>67</v>
       </c>
       <c r="H45" s="6">
-        <f t="shared" si="13"/>
-        <v>-363</v>
+        <f t="shared" si="14"/>
+        <v>-383</v>
       </c>
       <c r="I45" s="6">
-        <f t="shared" si="13"/>
-        <v>-363</v>
+        <f t="shared" si="14"/>
+        <v>-383</v>
       </c>
       <c r="J45" s="6">
-        <f t="shared" si="13"/>
-        <v>87</v>
+        <f t="shared" si="14"/>
+        <v>67</v>
       </c>
       <c r="K45" s="6">
-        <f t="shared" si="13"/>
-        <v>87</v>
+        <f t="shared" si="14"/>
+        <v>67</v>
       </c>
       <c r="L45" s="6">
-        <f t="shared" si="13"/>
-        <v>87</v>
+        <f t="shared" si="14"/>
+        <v>67</v>
       </c>
       <c r="M45" s="6">
-        <f t="shared" si="13"/>
-        <v>6447</v>
+        <f t="shared" si="14"/>
+        <v>6427</v>
       </c>
       <c r="N45" s="6">
-        <f t="shared" si="13"/>
-        <v>6504</v>
+        <f t="shared" si="14"/>
+        <v>6264</v>
       </c>
     </row>
     <row r="46" spans="1:14" s="1" customFormat="1">
       <c r="A46" s="9"/>
       <c r="B46" s="4">
         <f>IF(B$6=0,0,B45/B$6)</f>
-        <v>1.5818181818181818E-2</v>
+        <v>1.2181818181818183E-2</v>
       </c>
       <c r="C46" s="4">
-        <f t="shared" ref="C46:N46" si="14">IF(C$6=0,0,C45/C$6)</f>
-        <v>1.5818181818181818E-2</v>
+        <f t="shared" ref="C46:N46" si="15">IF(C$6=0,0,C45/C$6)</f>
+        <v>1.2181818181818183E-2</v>
       </c>
       <c r="D46" s="4">
-        <f t="shared" si="14"/>
-        <v>1.5818181818181818E-2</v>
+        <f t="shared" si="15"/>
+        <v>1.2181818181818183E-2</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" si="14"/>
-        <v>1.5818181818181818E-2</v>
+        <f t="shared" si="15"/>
+        <v>1.2181818181818183E-2</v>
       </c>
       <c r="F46" s="4">
-        <f t="shared" si="14"/>
-        <v>1.5818181818181818E-2</v>
+        <f t="shared" si="15"/>
+        <v>1.2181818181818183E-2</v>
       </c>
       <c r="G46" s="4">
-        <f t="shared" si="14"/>
-        <v>1.5818181818181818E-2</v>
+        <f t="shared" si="15"/>
+        <v>1.2181818181818183E-2</v>
       </c>
       <c r="H46" s="4">
-        <f t="shared" si="14"/>
-        <v>-6.6000000000000003E-2</v>
+        <f t="shared" si="15"/>
+        <v>-6.9636363636363635E-2</v>
       </c>
       <c r="I46" s="4">
-        <f t="shared" si="14"/>
-        <v>-6.6000000000000003E-2</v>
+        <f t="shared" si="15"/>
+        <v>-6.9636363636363635E-2</v>
       </c>
       <c r="J46" s="4">
-        <f t="shared" si="14"/>
-        <v>1.5818181818181818E-2</v>
+        <f t="shared" si="15"/>
+        <v>1.2181818181818183E-2</v>
       </c>
       <c r="K46" s="4">
-        <f t="shared" si="14"/>
-        <v>1.5818181818181818E-2</v>
+        <f t="shared" si="15"/>
+        <v>1.2181818181818183E-2</v>
       </c>
       <c r="L46" s="4">
-        <f t="shared" si="14"/>
-        <v>1.5818181818181818E-2</v>
+        <f t="shared" si="15"/>
+        <v>1.2181818181818183E-2</v>
       </c>
       <c r="M46" s="4">
-        <f t="shared" si="14"/>
-        <v>0.54359190556492409</v>
+        <f t="shared" si="15"/>
+        <v>0.54190556492411468</v>
       </c>
       <c r="N46" s="4">
-        <f t="shared" si="14"/>
-        <v>8.9883913764510784E-2</v>
+        <f t="shared" si="15"/>
+        <v>8.6567164179104483E-2</v>
       </c>
     </row>
     <row r="47" spans="1:14" s="1" customFormat="1">

</xml_diff>